<commit_message>
added number of families per region as of 2012
</commit_message>
<xml_diff>
--- a/Documentation/Population by Region.xlsx
+++ b/Documentation/Population by Region.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Desktop\IBMDESC-Poverty\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>Population</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Region</t>
   </si>
@@ -141,6 +138,15 @@
   </si>
   <si>
     <t>Autonomous Region in Muslim Mindanao</t>
+  </si>
+  <si>
+    <t>Population (2012)</t>
+  </si>
+  <si>
+    <t>Number of Families (2012)</t>
+  </si>
+  <si>
+    <t>Demographics</t>
   </si>
 </sst>
 </file>
@@ -194,10 +200,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -515,175 +528,256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4">
+        <v>2917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="4">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="4">
+        <v>3082</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="4">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="4">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="4">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="4">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="4">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="4">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="4">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="4">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="4">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="4">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
-        <v>38</v>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4">
+        <v>557</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>